<commit_message>
for some reason need to commit
</commit_message>
<xml_diff>
--- a/Testing Broad-Scale Interactions/Interaction_Matrix.xlsx
+++ b/Testing Broad-Scale Interactions/Interaction_Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radicinol\Desktop\R\Testing Broad-Scale Interactions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92aa253a0c32209f/Documents/GitHub/Microbial_Interactions/Testing Broad-Scale Interactions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF4A4CE-1175-422D-9381-B787F2E8D808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FCF4A4CE-1175-422D-9381-B787F2E8D808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{914359C4-218C-47A3-AF06-A308877C6F80}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03A45048-D6D3-4FA6-BE96-5E28A62A3FF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03A45048-D6D3-4FA6-BE96-5E28A62A3FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1080,13 +1080,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BB15BF-964D-4F39-ADC2-D0329E190B17}">
   <dimension ref="A1:C211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A191" sqref="A191:C191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>213</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>213</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>213</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>213</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>213</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>213</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>213</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>214</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>214</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>214</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>214</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>214</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>214</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>214</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>214</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>215</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>215</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>215</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>215</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>215</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>216</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>216</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>216</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>216</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>216</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>216</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>216</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>216</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>216</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>216</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>216</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>217</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>217</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>217</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>217</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>217</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>217</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>217</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>217</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>217</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>217</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>217</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>217</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>217</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>218</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>218</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>218</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>218</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>218</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>218</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>218</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>218</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>218</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>218</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>218</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>218</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>218</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>218</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>219</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>219</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>219</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>219</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>219</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>219</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>219</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>219</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>219</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>219</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>219</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>219</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>219</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>220</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>220</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>220</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>220</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>220</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>220</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>220</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>220</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>220</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>220</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>220</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>221</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>221</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>221</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>221</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>221</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>221</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>221</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>221</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>221</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>221</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>221</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>221</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>222</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>222</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>222</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>222</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>222</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>222</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>222</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>222</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>223</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>223</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>223</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>223</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>223</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>223</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>223</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>223</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>223</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>223</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>223</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>223</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>223</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>223</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>224</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>224</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>224</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>224</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>224</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>224</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>224</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>224</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>224</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>224</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>224</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>224</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>224</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>224</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>227</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>227</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>227</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>227</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>227</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>227</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>227</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>227</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>227</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>227</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>227</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>227</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>227</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>227</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>226</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>226</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>226</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>226</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>226</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>226</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>226</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>226</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>226</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>226</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>226</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>226</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>226</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>226</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>225</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>225</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>225</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>225</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>225</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>225</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>225</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>225</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>225</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>225</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>225</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>225</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>225</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>225</v>
       </c>

</xml_diff>